<commit_message>
Updated Queue to accomodate Disposition updates
</commit_message>
<xml_diff>
--- a/Data/Input/OfferLetterInput.xlsx
+++ b/Data/Input/OfferLetterInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C423CCB-6D02-42AD-9A43-43363C1E100F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1133EC2-F127-49F0-980D-1997A9C16140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OfferLetter" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Sl No#</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>C:\Users\55649C\Documents\Data\OMES Background Check Release HPABCD.pdf</t>
+  </si>
+  <si>
+    <t>DateOfHiring</t>
   </si>
 </sst>
 </file>
@@ -178,9 +181,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68576D6C-1169-468F-A26B-6582313AFCA5}" name="OfferLetterList" displayName="OfferLetterList" ref="A1:I7" totalsRowShown="0">
-  <autoFilter ref="A1:I7" xr:uid="{68576D6C-1169-468F-A26B-6582313AFCA5}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68576D6C-1169-468F-A26B-6582313AFCA5}" name="OfferLetterList" displayName="OfferLetterList" ref="A1:J7" totalsRowShown="0">
+  <autoFilter ref="A1:J7" xr:uid="{68576D6C-1169-468F-A26B-6582313AFCA5}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{586C7666-3997-4D89-99A1-CB65474E44F4}" name="Sl No#"/>
     <tableColumn id="2" xr3:uid="{A35A4DCB-1F64-46A7-9695-5CFE42088EE0}" name="Emp ID"/>
     <tableColumn id="3" xr3:uid="{902C02BA-CC07-42C7-882E-8081CEBCB06D}" name="JR.No"/>
@@ -189,6 +192,7 @@
     <tableColumn id="6" xr3:uid="{F77164E2-AFEF-4C70-BA3F-3ED91D6EA0A9}" name="Supervisor Email"/>
     <tableColumn id="7" xr3:uid="{D8DB6AB2-150E-420A-B3EC-78FB062ADCC6}" name="Annual Salary" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{2FD36DEF-2A9C-46A6-8DEA-84BF1D2B8726}" name="Status"/>
+    <tableColumn id="10" xr3:uid="{91753563-2E35-4CA4-9309-C8F7CCBCB710}" name="DateOfHiring"/>
     <tableColumn id="9" xr3:uid="{6AE0AA04-5A56-48FA-85B5-38DB34BEA72D}" name="Attachments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -458,26 +462,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.26953125" customWidth="1"/>
+    <col min="10" max="10" width="84.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,10 +508,13 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -531,11 +539,11 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -560,11 +568,11 @@
       <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -589,11 +597,11 @@
       <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -618,11 +626,11 @@
       <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -647,11 +655,11 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -676,7 +684,7 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to Variable Naming Convention
</commit_message>
<xml_diff>
--- a/Data/Input/OfferLetterInput.xlsx
+++ b/Data/Input/OfferLetterInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1133EC2-F127-49F0-980D-1997A9C16140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05566ED2-2604-4C40-99FE-81015FDF0CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,10 +117,10 @@
     <t>C:\Users\55649C\Documents\Data\Background Check Release Form.pdf</t>
   </si>
   <si>
-    <t>C:\Users\55649C\Documents\Data\OMES Background Check Release HPABCD.pdf</t>
-  </si>
-  <si>
     <t>DateOfHiring</t>
+  </si>
+  <si>
+    <t>C:\Users\55649C\Documents\Data\OMES Background Check Release HP.pdf</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -598,7 +598,7 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>